<commit_message>
Switched deck and card value.  Made skirmish a method.
</commit_message>
<xml_diff>
--- a/game_of_war.xlsx
+++ b/game_of_war.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="15460" yWindow="0" windowWidth="12800" windowHeight="26500" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="16360" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,10 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="24">
-  <si>
-    <t>Heart</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="25">
   <si>
     <t>J</t>
   </si>
@@ -36,15 +33,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>Spade</t>
-  </si>
-  <si>
-    <t>Clubs</t>
-  </si>
-  <si>
-    <t>Diamond</t>
-  </si>
-  <si>
     <t>modulo</t>
   </si>
   <si>
@@ -84,13 +72,28 @@
     <t>ask for count in lists</t>
   </si>
   <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Suit</t>
-  </si>
-  <si>
-    <t>Mod Value</t>
+    <t>S</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>Mod</t>
+  </si>
+  <si>
+    <t>Div</t>
+  </si>
+  <si>
+    <t>Card</t>
+  </si>
+  <si>
+    <t>Faces</t>
   </si>
 </sst>
 </file>
@@ -139,7 +142,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,8 +170,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -179,8 +188,14 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="33">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -194,6 +209,9 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -207,6 +225,9 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,862 +557,1075 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L54"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="6.83203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.6640625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="3.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1">
+    <row r="1" spans="1:13">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="5"/>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" s="1" customFormat="1">
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="1">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="1">
-        <v>2</v>
+      <c r="B2" s="4">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D2" s="1">
         <f>MOD(A2,13)</f>
         <v>0</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="1">
+        <f>QUOTIENT(A2,13)</f>
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="L2" s="3"/>
-    </row>
-    <row r="3" spans="1:12" s="1" customFormat="1">
+      <c r="M2" s="3"/>
+    </row>
+    <row r="3" spans="1:13">
       <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1">
-        <v>3</v>
+      <c r="B3" s="4">
+        <v>3</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D53" si="0">MOD(A3,13)</f>
         <v>1</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="E3" s="1">
+        <f t="shared" ref="E3:E53" si="1">QUOTIENT(A3,13)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="L3" s="3"/>
-    </row>
-    <row r="4" spans="1:12" s="1" customFormat="1">
+      <c r="M3" s="3"/>
+    </row>
+    <row r="4" spans="1:13">
       <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="1">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M4" s="3"/>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="4">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
-        <v>4</v>
-      </c>
-      <c r="D4" s="1">
-        <f t="shared" si="0"/>
-        <v>2</v>
-      </c>
-      <c r="L4" s="3"/>
-    </row>
-    <row r="5" spans="1:12" s="1" customFormat="1">
-      <c r="A5" s="1">
-        <v>3</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C5" s="1">
-        <v>5</v>
+      <c r="C5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="L5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" s="1" customFormat="1">
+      <c r="E5" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M5" s="3"/>
+    </row>
+    <row r="6" spans="1:13">
       <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C6" s="1">
+      <c r="B6" s="4">
         <v>6</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" s="1" customFormat="1">
+      <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="3"/>
+    </row>
+    <row r="7" spans="1:13">
       <c r="A7" s="1">
         <v>5</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="4">
+        <v>7</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C7" s="1">
-        <v>7</v>
-      </c>
-      <c r="D7" s="1">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="L7" s="3"/>
-    </row>
-    <row r="8" spans="1:12" s="1" customFormat="1">
+      <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M7" s="3"/>
+    </row>
+    <row r="8" spans="1:13">
       <c r="A8" s="1">
         <v>6</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" s="1">
+      <c r="B8" s="4">
         <v>8</v>
       </c>
+      <c r="C8" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="L8" s="3"/>
-    </row>
-    <row r="9" spans="1:12" s="1" customFormat="1">
+      <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="1:13">
       <c r="A9" s="1">
         <v>7</v>
       </c>
-      <c r="B9" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="1">
+      <c r="B9" s="4">
         <v>9</v>
       </c>
+      <c r="C9" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="F9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" s="1" customFormat="1">
+      <c r="E9" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
       <c r="A10" s="1">
         <v>8</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C10" s="1">
+      <c r="B10" s="4">
         <v>10</v>
       </c>
+      <c r="C10" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" s="1" customFormat="1">
+      <c r="E10" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
       <c r="A11" s="1">
         <v>9</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>5</v>
+      <c r="B11" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1</v>
+        <v>17</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" s="1" customFormat="1">
+      <c r="E11" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
       <c r="A12" s="1">
         <v>10</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>5</v>
+      <c r="B12" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" s="1" customFormat="1">
+      <c r="E12" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
       <c r="A13" s="1">
         <v>11</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>5</v>
+      <c r="B13" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" s="1" customFormat="1">
+      <c r="E13" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
       <c r="A14" s="1">
         <v>12</v>
       </c>
-      <c r="B14" s="1" t="s">
-        <v>5</v>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" s="1" customFormat="1">
+      <c r="E14" s="1">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
       <c r="A15" s="1">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2</v>
+      <c r="B15" s="4">
+        <v>2</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" s="1" customFormat="1">
+      <c r="E15" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3</v>
+      <c r="B16" s="4">
+        <v>3</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" s="1" customFormat="1">
+      <c r="E16" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1">
         <v>15</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="1">
+      <c r="B17" s="4">
         <v>4</v>
       </c>
+      <c r="C17" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" s="1" customFormat="1">
+      <c r="E17" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" s="1">
         <v>16</v>
       </c>
-      <c r="B18" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="1">
+      <c r="B18" s="4">
         <v>5</v>
       </c>
+      <c r="C18" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" s="1" customFormat="1">
+      <c r="E18" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" s="1">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="1">
+      <c r="B19" s="4">
         <v>6</v>
       </c>
+      <c r="C19" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" s="1" customFormat="1">
+      <c r="E19" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" s="1">
         <v>18</v>
       </c>
-      <c r="B20" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="1">
+      <c r="B20" s="4">
         <v>7</v>
       </c>
+      <c r="C20" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" s="1" customFormat="1">
+      <c r="E20" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1">
         <v>19</v>
       </c>
-      <c r="B21" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="1">
+      <c r="B21" s="4">
         <v>8</v>
       </c>
+      <c r="C21" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" s="1" customFormat="1">
+      <c r="E21" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" s="1">
         <v>20</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="1">
+      <c r="B22" s="4">
         <v>9</v>
       </c>
+      <c r="C22" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" s="1" customFormat="1">
+      <c r="E22" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1">
         <v>21</v>
       </c>
-      <c r="B23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1">
+      <c r="B23" s="4">
         <v>10</v>
       </c>
+      <c r="C23" s="1" t="s">
+        <v>18</v>
+      </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" s="1" customFormat="1">
+      <c r="E23" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" s="1">
         <v>22</v>
       </c>
-      <c r="B24" s="1" t="s">
+      <c r="B24" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" s="1" customFormat="1">
+      <c r="E24" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1">
         <v>23</v>
       </c>
-      <c r="B25" s="1" t="s">
-        <v>0</v>
+      <c r="B25" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" s="1" customFormat="1">
+      <c r="E25" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" s="1">
         <v>24</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>0</v>
+      <c r="B26" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" s="1" customFormat="1">
+      <c r="E26" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1">
         <v>25</v>
       </c>
-      <c r="B27" s="1" t="s">
-        <v>0</v>
+      <c r="B27" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" s="1" customFormat="1">
+      <c r="E27" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" s="1">
         <v>26</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C28" s="1">
-        <v>2</v>
+      <c r="B28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" s="1" customFormat="1">
+      <c r="E28" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" s="1">
         <v>27</v>
       </c>
-      <c r="B29" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C29" s="1">
-        <v>3</v>
+      <c r="B29" s="4">
+        <v>3</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" s="1" customFormat="1">
+      <c r="E29" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" s="1">
         <v>28</v>
       </c>
-      <c r="B30" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C30" s="1">
+      <c r="B30" s="4">
         <v>4</v>
       </c>
+      <c r="C30" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" s="1" customFormat="1">
+      <c r="E30" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" s="1">
         <v>29</v>
       </c>
-      <c r="B31" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C31" s="1">
+      <c r="B31" s="4">
         <v>5</v>
       </c>
+      <c r="C31" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" s="1" customFormat="1">
+      <c r="E31" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" s="1">
         <v>30</v>
       </c>
-      <c r="B32" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C32" s="1">
+      <c r="B32" s="4">
         <v>6</v>
       </c>
+      <c r="C32" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" s="1" customFormat="1">
+      <c r="E32" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" s="1">
         <v>31</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="4">
         <v>7</v>
       </c>
-      <c r="C33" s="1">
-        <v>7</v>
+      <c r="C33" s="1" t="s">
+        <v>19</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" s="1" customFormat="1">
+      <c r="E33" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B34" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C34" s="1">
+      <c r="B34" s="4">
         <v>8</v>
       </c>
+      <c r="C34" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" s="1" customFormat="1">
+      <c r="E34" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" s="1">
         <v>33</v>
       </c>
-      <c r="B35" s="1" t="s">
+      <c r="B35" s="4">
+        <v>9</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35" s="1">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C35" s="1">
-        <v>9</v>
-      </c>
-      <c r="D35" s="1">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" s="1" customFormat="1">
+      <c r="E35" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" s="1">
         <v>34</v>
       </c>
-      <c r="B36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C36" s="1">
+      <c r="B36" s="4">
         <v>10</v>
       </c>
+      <c r="C36" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" s="1" customFormat="1">
+      <c r="E36" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" s="1">
         <v>35</v>
       </c>
-      <c r="B37" s="1" t="s">
-        <v>7</v>
+      <c r="B37" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" s="1" customFormat="1">
+      <c r="E37" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" s="1">
         <v>36</v>
       </c>
-      <c r="B38" s="1" t="s">
-        <v>7</v>
+      <c r="B38" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" s="1" customFormat="1">
+      <c r="E38" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" s="1">
         <v>37</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>7</v>
+      <c r="B39" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" s="1" customFormat="1">
+      <c r="E39" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" s="1">
         <v>38</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>7</v>
+      <c r="B40" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" s="1" customFormat="1">
+      <c r="E40" s="1">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" s="1">
         <v>39</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C41" s="1">
-        <v>2</v>
+      <c r="B41" s="4">
+        <v>2</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" s="1" customFormat="1">
+      <c r="E41" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" s="1">
         <v>40</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C42" s="1">
-        <v>3</v>
+      <c r="B42" s="4">
+        <v>3</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" s="1" customFormat="1">
+      <c r="E42" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" s="1">
         <v>41</v>
       </c>
-      <c r="B43" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="1">
+      <c r="B43" s="4">
         <v>4</v>
       </c>
+      <c r="C43" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D43" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" s="1" customFormat="1">
+      <c r="E43" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" s="1">
         <v>42</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C44" s="1">
+      <c r="B44" s="4">
         <v>5</v>
       </c>
+      <c r="C44" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D44" s="1">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" s="1" customFormat="1">
+      <c r="E44" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1">
         <v>43</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B45" s="4">
         <v>6</v>
       </c>
-      <c r="C45" s="1">
-        <v>6</v>
+      <c r="C45" s="1" t="s">
+        <v>20</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" s="1" customFormat="1">
+      <c r="E45" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1">
         <v>44</v>
       </c>
-      <c r="B46" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C46" s="1">
+      <c r="B46" s="4">
         <v>7</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D46" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" s="1" customFormat="1">
+      <c r="E46" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" s="1">
         <v>45</v>
       </c>
-      <c r="B47" s="1" t="s">
+      <c r="B47" s="4">
+        <v>8</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D47" s="1">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C47" s="1">
-        <v>8</v>
-      </c>
-      <c r="D47" s="1">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" s="1" customFormat="1">
+      <c r="E47" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1">
         <v>46</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C48" s="1">
+      <c r="B48" s="4">
         <v>9</v>
       </c>
+      <c r="C48" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D48" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" s="1" customFormat="1">
+      <c r="E48" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" s="1">
         <v>47</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C49" s="1">
+      <c r="B49" s="4">
         <v>10</v>
       </c>
+      <c r="C49" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D49" s="1">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" s="1" customFormat="1">
+      <c r="E49" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" s="1">
         <v>48</v>
       </c>
-      <c r="B50" s="1" t="s">
-        <v>6</v>
+      <c r="B50" s="4" t="s">
+        <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" s="1" customFormat="1">
+      <c r="E50" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" s="1">
         <v>49</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>6</v>
+      <c r="B51" s="4" t="s">
+        <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" s="1" customFormat="1">
+      <c r="E51" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" s="1">
         <v>50</v>
       </c>
-      <c r="B52" s="1" t="s">
-        <v>6</v>
+      <c r="B52" s="4" t="s">
+        <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" s="1" customFormat="1">
+      <c r="E52" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" s="1">
         <v>51</v>
       </c>
-      <c r="B53" s="1" t="s">
-        <v>6</v>
+      <c r="B53" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>4</v>
+        <v>20</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" s="1" customFormat="1"/>
+      <c r="E53" s="1">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Change card class to use index int
</commit_message>
<xml_diff>
--- a/game_of_war.xlsx
+++ b/game_of_war.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="16360" tabRatio="500"/>
+    <workbookView xWindow="20800" yWindow="0" windowWidth="8000" windowHeight="16460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -106,6 +106,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -142,8 +143,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -195,7 +204,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -212,6 +221,10 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -228,6 +241,10 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -559,8 +576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="175" zoomScaleNormal="175" zoomScalePageLayoutView="175" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -596,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D2" s="1">
         <f>MOD(A2,13)</f>
@@ -625,7 +642,7 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D3" s="1">
         <f t="shared" ref="D3:D53" si="0">MOD(A3,13)</f>
@@ -654,7 +671,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" s="1">
         <f t="shared" si="0"/>
@@ -674,7 +691,7 @@
         <v>5</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D5" s="1">
         <f t="shared" si="0"/>
@@ -697,7 +714,7 @@
         <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D6" s="1">
         <f t="shared" si="0"/>
@@ -720,7 +737,7 @@
         <v>7</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D7" s="1">
         <f t="shared" si="0"/>
@@ -743,7 +760,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="1">
         <f t="shared" si="0"/>
@@ -766,7 +783,7 @@
         <v>9</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D9" s="1">
         <f t="shared" si="0"/>
@@ -788,7 +805,7 @@
         <v>10</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D10" s="1">
         <f t="shared" si="0"/>
@@ -810,7 +827,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D11" s="1">
         <f t="shared" si="0"/>
@@ -832,7 +849,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D12" s="1">
         <f t="shared" si="0"/>
@@ -851,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D13" s="1">
         <f t="shared" si="0"/>
@@ -870,7 +887,7 @@
         <v>3</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D14" s="1">
         <f t="shared" si="0"/>
@@ -889,7 +906,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D15" s="1">
         <f t="shared" si="0"/>
@@ -908,7 +925,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D16" s="1">
         <f t="shared" si="0"/>
@@ -927,7 +944,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D17" s="1">
         <f t="shared" si="0"/>
@@ -946,7 +963,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D18" s="1">
         <f t="shared" si="0"/>
@@ -965,7 +982,7 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D19" s="1">
         <f t="shared" si="0"/>
@@ -984,7 +1001,7 @@
         <v>7</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D20" s="1">
         <f t="shared" si="0"/>
@@ -1003,7 +1020,7 @@
         <v>8</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D21" s="1">
         <f t="shared" si="0"/>
@@ -1022,7 +1039,7 @@
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D22" s="1">
         <f t="shared" si="0"/>
@@ -1041,7 +1058,7 @@
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D23" s="1">
         <f t="shared" si="0"/>
@@ -1060,7 +1077,7 @@
         <v>0</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D24" s="1">
         <f t="shared" si="0"/>
@@ -1079,7 +1096,7 @@
         <v>1</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D25" s="1">
         <f t="shared" si="0"/>
@@ -1098,7 +1115,7 @@
         <v>2</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D26" s="1">
         <f t="shared" si="0"/>
@@ -1117,7 +1134,7 @@
         <v>3</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D27" s="1">
         <f t="shared" si="0"/>
@@ -1136,7 +1153,7 @@
         <v>2</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D28" s="1">
         <f t="shared" si="0"/>
@@ -1155,7 +1172,7 @@
         <v>3</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D29" s="1">
         <f t="shared" si="0"/>
@@ -1174,7 +1191,7 @@
         <v>4</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D30" s="1">
         <f t="shared" si="0"/>
@@ -1193,7 +1210,7 @@
         <v>5</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D31" s="1">
         <f t="shared" si="0"/>
@@ -1212,7 +1229,7 @@
         <v>6</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D32" s="1">
         <f t="shared" si="0"/>
@@ -1231,7 +1248,7 @@
         <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D33" s="1">
         <f t="shared" si="0"/>
@@ -1250,7 +1267,7 @@
         <v>8</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D34" s="1">
         <f t="shared" si="0"/>
@@ -1269,7 +1286,7 @@
         <v>9</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D35" s="1">
         <f t="shared" si="0"/>
@@ -1288,7 +1305,7 @@
         <v>10</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D36" s="1">
         <f t="shared" si="0"/>
@@ -1307,7 +1324,7 @@
         <v>0</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D37" s="1">
         <f t="shared" si="0"/>
@@ -1326,7 +1343,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D38" s="1">
         <f t="shared" si="0"/>
@@ -1345,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D39" s="1">
         <f t="shared" si="0"/>
@@ -1364,7 +1381,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D40" s="1">
         <f t="shared" si="0"/>
@@ -1383,7 +1400,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D41" s="1">
         <f t="shared" si="0"/>
@@ -1402,7 +1419,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D42" s="1">
         <f t="shared" si="0"/>
@@ -1421,7 +1438,7 @@
         <v>4</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D43" s="1">
         <f t="shared" si="0"/>
@@ -1440,7 +1457,7 @@
         <v>5</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D44" s="1">
         <f t="shared" si="0"/>
@@ -1459,7 +1476,7 @@
         <v>6</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D45" s="1">
         <f t="shared" si="0"/>
@@ -1478,7 +1495,7 @@
         <v>7</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D46" s="1">
         <f t="shared" si="0"/>
@@ -1497,7 +1514,7 @@
         <v>8</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D47" s="1">
         <f t="shared" si="0"/>
@@ -1516,7 +1533,7 @@
         <v>9</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D48" s="1">
         <f t="shared" si="0"/>
@@ -1535,7 +1552,7 @@
         <v>10</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D49" s="1">
         <f t="shared" si="0"/>
@@ -1554,7 +1571,7 @@
         <v>0</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D50" s="1">
         <f t="shared" si="0"/>
@@ -1573,7 +1590,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D51" s="1">
         <f t="shared" si="0"/>
@@ -1592,7 +1609,7 @@
         <v>2</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D52" s="1">
         <f t="shared" si="0"/>
@@ -1611,7 +1628,7 @@
         <v>3</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D53" s="1">
         <f t="shared" si="0"/>

</xml_diff>